<commit_message>
Add print statement to schedule function
</commit_message>
<xml_diff>
--- a/static/schedule-instructores/Horario 1-2024 - DANIEL DAVID BENAVIDES SÁNCHEZ.xlsx
+++ b/static/schedule-instructores/Horario 1-2024 - DANIEL DAVID BENAVIDES SÁNCHEZ.xlsx
@@ -66,7 +66,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -76,6 +76,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -471,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -918,6 +922,148 @@
       <c r="F25" s="4" t="n"/>
       <c r="G25" s="4" t="n"/>
     </row>
+    <row r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>Ficha</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>Trimestre</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>Palabra clave</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>Norma de Competencia (Sofíaplus)</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>Competencia</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>RAP</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>2771132 A</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>TEC. PROGRAMACIÓN</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
+        <is>
+          <t>Proyecto 2 + Pruebas (Tc.)</t>
+        </is>
+      </c>
+      <c r="E28" s="6" t="inlineStr">
+        <is>
+          <t>Desarrollar la solución de software de acuerdo con el diseño y metodologías de desarrollo.</t>
+        </is>
+      </c>
+      <c r="F28" s="6" t="inlineStr">
+        <is>
+          <t>Desarrollo de la solución de software.</t>
+        </is>
+      </c>
+      <c r="G28" s="6" t="inlineStr">
+        <is>
+          <t>Codificar el software empleando el lenguaje de programación seleccionado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>2821717 A</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>ADSO</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>CSS, HTML</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>Desarrollar la solución de software de acuerdo con el diseño y metodologías de desarrollo.</t>
+        </is>
+      </c>
+      <c r="F29" s="6" t="inlineStr">
+        <is>
+          <t>Construcción del software.</t>
+        </is>
+      </c>
+      <c r="G29" s="6" t="inlineStr">
+        <is>
+          <t>Crear componentes front-end del software de acuerdo con el diseño.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>2617472 A</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>ADSO</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
+        <is>
+          <t>Python (Machine Learning + Big Data)</t>
+        </is>
+      </c>
+      <c r="E30" s="6" t="inlineStr">
+        <is>
+          <t>Desarrollar la solución de software de acuerdo con el diseño y metodologías de desarrollo.</t>
+        </is>
+      </c>
+      <c r="F30" s="6" t="inlineStr">
+        <is>
+          <t>Construcción del software.</t>
+        </is>
+      </c>
+      <c r="G30" s="6" t="inlineStr">
+        <is>
+          <t>Codificar el software de acuerdo con el diseño establecido.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update instructor hours variable in dashboard.html
</commit_message>
<xml_diff>
--- a/static/schedule-instructores/Horario 1-2024 - DANIEL DAVID BENAVIDES SÁNCHEZ.xlsx
+++ b/static/schedule-instructores/Horario 1-2024 - DANIEL DAVID BENAVIDES SÁNCHEZ.xlsx
@@ -475,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G30"/>
+  <dimension ref="A2:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,7 +607,13 @@
  803</t>
         </is>
       </c>
-      <c r="F9" s="3" t="inlineStr"/>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>Matemáticas 
+ 2821717 A 
+ 802</t>
+        </is>
+      </c>
       <c r="G9" s="3" t="inlineStr"/>
     </row>
     <row r="10">
@@ -644,7 +650,13 @@
  803</t>
         </is>
       </c>
-      <c r="F10" s="3" t="inlineStr"/>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>Matemáticas 
+ 2821717 A 
+ 802</t>
+        </is>
+      </c>
       <c r="G10" s="3" t="inlineStr"/>
     </row>
     <row r="11">
@@ -1064,6 +1076,41 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>2821717 A</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>ADSO</t>
+        </is>
+      </c>
+      <c r="D31" s="6" t="inlineStr">
+        <is>
+          <t>Matemáticas</t>
+        </is>
+      </c>
+      <c r="E31" s="6" t="inlineStr">
+        <is>
+          <t>Razonar cuantitativamente frente a situaciones susceptibles de ser abordadas de manera matemática en contextos laborales, sociales y personales.</t>
+        </is>
+      </c>
+      <c r="F31" s="6" t="inlineStr">
+        <is>
+          <t>Matemáticas</t>
+        </is>
+      </c>
+      <c r="G31" s="6" t="inlineStr">
+        <is>
+          <t>Identificar modelos matemáticos de acuerdo con los requerimientos del problema planteado en contextos sociales y productivo.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>